<commit_message>
Added all missing footprints, first realistic layout
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/IRIS2_PCB_FrontPlate/docs/Calculations.xlsx
+++ b/IRIS2/01-Design/IRIS2_PCB_FrontPlate/docs/Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\IRIS2_PCB_FrontPlate\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D877E109-81D0-4140-94F9-5B9736D16A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714C59AD-F4F4-41EF-8B49-353E4877F35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>R</t>
   </si>
@@ -375,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,6 +432,38 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <f>28-1.55</f>
+        <v>26.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <f>B7/B8</f>
+        <v>2645</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>